<commit_message>
Add speedup of FEE
</commit_message>
<xml_diff>
--- a/S32K3/S32K3xx_memory_map.xlsx
+++ b/S32K3/S32K3xx_memory_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf93503\Documents\S32K3\iomux\April2024\READY_TO_SEND\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter_chen.WTMEC\Documents\Projects\NXPMCUFAQ\S32K3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180E7BD-79FC-4F5F-BD19-E3A80D79A132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD394281-41BD-4434-A7CE-D2D2D87C6103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{01270DDA-191B-4F02-B2B3-5014FCE039BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01270DDA-191B-4F02-B2B3-5014FCE039BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Memories" sheetId="43" r:id="rId1"/>
@@ -2744,7 +2744,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2752,70 +2752,70 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2901,6 +2901,12 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3244,6 +3250,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3262,12 +3274,6 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="4" xfId="109" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="110">
     <cellStyle name="Excel Built-in Normal" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3276,7 +3282,6 @@
     <cellStyle name="Hyperlink 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Light Gray Border" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Light Gray row border" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 2 2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
@@ -3380,6 +3385,7 @@
     <cellStyle name="標準 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
     <cellStyle name="標準 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
     <cellStyle name="標準 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -3747,46 +3753,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398203C9-8515-42E4-880B-3A5DAA1437D6}">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="12"/>
-    <col min="4" max="4" width="35.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="21" width="8.88671875" style="13"/>
+    <col min="2" max="2" width="17.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="12"/>
+    <col min="4" max="4" width="35.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="21" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="31" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="33"/>
-    </row>
-    <row r="2" spans="1:21" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="35"/>
+    </row>
+    <row r="2" spans="1:21" s="3" customFormat="1" ht="45.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>487</v>
       </c>
@@ -3851,7 +3857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>415</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>415</v>
       </c>
@@ -3961,7 +3967,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>415</v>
       </c>
@@ -4004,7 +4010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>415</v>
       </c>
@@ -4041,7 +4047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>416</v>
       </c>
@@ -4078,7 +4084,7 @@
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
     </row>
-    <row r="8" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>417</v>
       </c>
@@ -4113,7 +4119,7 @@
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
     </row>
-    <row r="9" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>416</v>
       </c>
@@ -4160,7 +4166,7 @@
       <c r="T9" s="8"/>
       <c r="U9" s="8"/>
     </row>
-    <row r="10" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>418</v>
       </c>
@@ -4205,7 +4211,7 @@
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
     </row>
-    <row r="11" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>419</v>
       </c>
@@ -4244,7 +4250,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>420</v>
       </c>
@@ -4283,7 +4289,7 @@
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
     </row>
-    <row r="13" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>416</v>
       </c>
@@ -4328,7 +4334,7 @@
       </c>
       <c r="U13" s="8"/>
     </row>
-    <row r="14" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>419</v>
       </c>
@@ -4373,7 +4379,7 @@
       </c>
       <c r="U14" s="8"/>
     </row>
-    <row r="15" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>421</v>
       </c>
@@ -4418,7 +4424,7 @@
       </c>
       <c r="U15" s="8"/>
     </row>
-    <row r="16" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>422</v>
       </c>
@@ -4461,7 +4467,7 @@
       </c>
       <c r="U16" s="8"/>
     </row>
-    <row r="17" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>416</v>
       </c>
@@ -4496,7 +4502,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>418</v>
       </c>
@@ -4531,7 +4537,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>419</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>421</v>
       </c>
@@ -4601,7 +4607,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>422</v>
       </c>
@@ -4636,7 +4642,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>423</v>
       </c>
@@ -4671,7 +4677,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>424</v>
       </c>
@@ -4706,7 +4712,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>425</v>
       </c>
@@ -4741,7 +4747,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>426</v>
       </c>
@@ -4786,7 +4792,7 @@
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
     </row>
-    <row r="26" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>426</v>
       </c>
@@ -4837,7 +4843,7 @@
       </c>
       <c r="U26" s="8"/>
     </row>
-    <row r="27" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>426</v>
       </c>
@@ -4872,7 +4878,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>427</v>
       </c>
@@ -4937,7 +4943,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>428</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>429</v>
       </c>
@@ -5031,7 +5037,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>430</v>
       </c>
@@ -5068,7 +5074,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>431</v>
       </c>
@@ -5131,7 +5137,7 @@
       </c>
       <c r="U32" s="8"/>
     </row>
-    <row r="33" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>431</v>
       </c>
@@ -5166,7 +5172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>432</v>
       </c>
@@ -5231,7 +5237,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>432</v>
       </c>
@@ -5276,7 +5282,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>432</v>
       </c>
@@ -5319,7 +5325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>432</v>
       </c>
@@ -5356,7 +5362,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>433</v>
       </c>
@@ -5407,7 +5413,7 @@
       <c r="T38" s="8"/>
       <c r="U38" s="8"/>
     </row>
-    <row r="39" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>434</v>
       </c>
@@ -5446,7 +5452,7 @@
       <c r="T39" s="8"/>
       <c r="U39" s="8"/>
     </row>
-    <row r="40" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>433</v>
       </c>
@@ -5491,7 +5497,7 @@
       </c>
       <c r="U40" s="8"/>
     </row>
-    <row r="41" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>435</v>
       </c>
@@ -5536,7 +5542,7 @@
       </c>
       <c r="U41" s="8"/>
     </row>
-    <row r="42" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>436</v>
       </c>
@@ -5581,7 +5587,7 @@
       </c>
       <c r="U42" s="8"/>
     </row>
-    <row r="43" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>433</v>
       </c>
@@ -5616,7 +5622,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>436</v>
       </c>
@@ -5651,7 +5657,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>437</v>
       </c>
@@ -5686,7 +5692,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>438</v>
       </c>
@@ -5721,7 +5727,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>439</v>
       </c>
@@ -5786,7 +5792,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>440</v>
       </c>
@@ -5833,7 +5839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>441</v>
       </c>
@@ -5880,7 +5886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>442</v>
       </c>
@@ -5917,7 +5923,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>443</v>
       </c>
@@ -5982,7 +5988,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>444</v>
       </c>
@@ -6047,7 +6053,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>445</v>
       </c>
@@ -6106,7 +6112,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>446</v>
       </c>
@@ -6143,7 +6149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>447</v>
       </c>
@@ -6202,7 +6208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>448</v>
       </c>
@@ -6261,7 +6267,7 @@
         <v>131072</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>449</v>
       </c>
@@ -6326,7 +6332,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>63</v>
       </c>
@@ -6353,7 +6359,7 @@
         <v>256</v>
       </c>
       <c r="L58" s="11">
-        <v>512</v>
+        <v>416</v>
       </c>
       <c r="M58" s="11">
         <v>512</v>
@@ -6389,6 +6395,7 @@
     <mergeCell ref="F1:U1"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -6398,25 +6405,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC8F81-7F97-4E33-8AE4-FE56471D62CF}">
   <dimension ref="A1:Z193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="30" customWidth="1"/>
-    <col min="10" max="25" width="8.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="30" customWidth="1"/>
+    <col min="10" max="25" width="8.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="45.75" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>490</v>
       </c>
@@ -6493,7 +6500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>67</v>
       </c>
@@ -6570,7 +6577,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>75</v>
       </c>
@@ -6645,7 +6652,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>69</v>
       </c>
@@ -6722,7 +6729,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>71</v>
       </c>
@@ -6797,7 +6804,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>74</v>
       </c>
@@ -6872,7 +6879,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>77</v>
       </c>
@@ -6947,7 +6954,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>79</v>
       </c>
@@ -7022,7 +7029,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>81</v>
       </c>
@@ -7097,7 +7104,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>83</v>
       </c>
@@ -7172,7 +7179,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>85</v>
       </c>
@@ -7247,7 +7254,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>87</v>
       </c>
@@ -7322,7 +7329,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>89</v>
       </c>
@@ -7397,7 +7404,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>91</v>
       </c>
@@ -7472,7 +7479,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>93</v>
       </c>
@@ -7547,7 +7554,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>95</v>
       </c>
@@ -7622,7 +7629,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>97</v>
       </c>
@@ -7697,7 +7704,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>99</v>
       </c>
@@ -7772,7 +7779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>101</v>
       </c>
@@ -7847,7 +7854,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>101</v>
       </c>
@@ -7922,7 +7929,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>103</v>
       </c>
@@ -7997,7 +8004,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>103</v>
       </c>
@@ -8072,7 +8079,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>107</v>
       </c>
@@ -8147,7 +8154,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>107</v>
       </c>
@@ -8222,7 +8229,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>110</v>
       </c>
@@ -8299,7 +8306,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>112</v>
       </c>
@@ -8376,7 +8383,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>127</v>
       </c>
@@ -8453,7 +8460,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>148</v>
       </c>
@@ -8530,7 +8537,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>153</v>
       </c>
@@ -8607,7 +8614,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>155</v>
       </c>
@@ -8684,7 +8691,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>157</v>
       </c>
@@ -8761,7 +8768,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>159</v>
       </c>
@@ -8838,7 +8845,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>161</v>
       </c>
@@ -8915,7 +8922,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>163</v>
       </c>
@@ -8992,7 +8999,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>115</v>
       </c>
@@ -9069,7 +9076,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>117</v>
       </c>
@@ -9146,7 +9153,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>119</v>
       </c>
@@ -9223,7 +9230,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>121</v>
       </c>
@@ -9300,7 +9307,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>123</v>
       </c>
@@ -9377,7 +9384,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>125</v>
       </c>
@@ -9454,7 +9461,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
         <v>128</v>
       </c>
@@ -9529,7 +9536,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>129</v>
       </c>
@@ -9604,7 +9611,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="s">
         <v>130</v>
       </c>
@@ -9679,7 +9686,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="27" t="s">
         <v>131</v>
       </c>
@@ -9754,7 +9761,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
         <v>132</v>
       </c>
@@ -9829,7 +9836,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>133</v>
       </c>
@@ -9904,7 +9911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>134</v>
       </c>
@@ -9979,7 +9986,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>135</v>
       </c>
@@ -10054,7 +10061,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>136</v>
       </c>
@@ -10129,7 +10136,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>138</v>
       </c>
@@ -10206,7 +10213,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="23" t="s">
         <v>140</v>
       </c>
@@ -10283,7 +10290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>142</v>
       </c>
@@ -10358,7 +10365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>144</v>
       </c>
@@ -10433,7 +10440,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>146</v>
       </c>
@@ -10510,7 +10517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>149</v>
       </c>
@@ -10585,7 +10592,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>151</v>
       </c>
@@ -10660,7 +10667,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>165</v>
       </c>
@@ -10737,7 +10744,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>167</v>
       </c>
@@ -10814,7 +10821,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>169</v>
       </c>
@@ -10889,7 +10896,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>171</v>
       </c>
@@ -10966,7 +10973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>173</v>
       </c>
@@ -11041,7 +11048,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>173</v>
       </c>
@@ -11116,7 +11123,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>175</v>
       </c>
@@ -11191,7 +11198,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
         <v>175</v>
       </c>
@@ -11266,7 +11273,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
         <v>177</v>
       </c>
@@ -11341,7 +11348,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="17" t="s">
         <v>177</v>
       </c>
@@ -11416,7 +11423,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
         <v>178</v>
       </c>
@@ -11491,7 +11498,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
         <v>180</v>
       </c>
@@ -11568,7 +11575,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
         <v>182</v>
       </c>
@@ -11643,7 +11650,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
         <v>184</v>
       </c>
@@ -11720,7 +11727,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
         <v>187</v>
       </c>
@@ -11795,7 +11802,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
         <v>189</v>
       </c>
@@ -11870,7 +11877,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
         <v>191</v>
       </c>
@@ -11945,7 +11952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
         <v>193</v>
       </c>
@@ -12020,7 +12027,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
         <v>195</v>
       </c>
@@ -12097,7 +12104,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
         <v>197</v>
       </c>
@@ -12174,7 +12181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
         <v>199</v>
       </c>
@@ -12251,7 +12258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
         <v>201</v>
       </c>
@@ -12328,7 +12335,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="17" t="s">
         <v>203</v>
       </c>
@@ -12405,7 +12412,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
         <v>205</v>
       </c>
@@ -12482,7 +12489,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
         <v>207</v>
       </c>
@@ -12559,7 +12566,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="17" t="s">
         <v>209</v>
       </c>
@@ -12634,7 +12641,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
         <v>211</v>
       </c>
@@ -12709,7 +12716,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
         <v>211</v>
       </c>
@@ -12784,7 +12791,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
         <v>213</v>
       </c>
@@ -12859,7 +12866,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
         <v>215</v>
       </c>
@@ -12934,7 +12941,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
         <v>216</v>
       </c>
@@ -13009,7 +13016,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
         <v>217</v>
       </c>
@@ -13084,7 +13091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
         <v>218</v>
       </c>
@@ -13159,7 +13166,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
         <v>219</v>
       </c>
@@ -13234,7 +13241,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
         <v>220</v>
       </c>
@@ -13309,7 +13316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
         <v>221</v>
       </c>
@@ -13384,7 +13391,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
         <v>222</v>
       </c>
@@ -13459,7 +13466,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
         <v>223</v>
       </c>
@@ -13534,7 +13541,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
         <v>413</v>
       </c>
@@ -13609,7 +13616,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
         <v>226</v>
       </c>
@@ -13684,7 +13691,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
         <v>228</v>
       </c>
@@ -13759,7 +13766,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="98" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
         <v>230</v>
       </c>
@@ -13834,7 +13841,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
         <v>232</v>
       </c>
@@ -13909,7 +13916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
         <v>234</v>
       </c>
@@ -13984,7 +13991,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
         <v>236</v>
       </c>
@@ -14059,7 +14066,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
         <v>238</v>
       </c>
@@ -14134,7 +14141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
         <v>240</v>
       </c>
@@ -14209,7 +14216,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
         <v>242</v>
       </c>
@@ -14284,7 +14291,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
         <v>242</v>
       </c>
@@ -14359,7 +14366,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
         <v>244</v>
       </c>
@@ -14434,7 +14441,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
         <v>246</v>
       </c>
@@ -14509,7 +14516,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="108" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
         <v>248</v>
       </c>
@@ -14584,7 +14591,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
         <v>250</v>
       </c>
@@ -14659,7 +14666,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
         <v>252</v>
       </c>
@@ -14734,7 +14741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
         <v>254</v>
       </c>
@@ -14809,7 +14816,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
         <v>256</v>
       </c>
@@ -14884,7 +14891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
         <v>258</v>
       </c>
@@ -14959,7 +14966,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
         <v>260</v>
       </c>
@@ -15034,7 +15041,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="19" t="s">
         <v>262</v>
       </c>
@@ -15109,7 +15116,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
         <v>280</v>
       </c>
@@ -15186,7 +15193,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
         <v>282</v>
       </c>
@@ -15261,7 +15268,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
         <v>284</v>
       </c>
@@ -15336,7 +15343,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
         <v>264</v>
       </c>
@@ -15411,7 +15418,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
         <v>266</v>
       </c>
@@ -15486,7 +15493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="121" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
         <v>268</v>
       </c>
@@ -15561,7 +15568,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
         <v>270</v>
       </c>
@@ -15636,7 +15643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="123" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
         <v>272</v>
       </c>
@@ -15711,7 +15718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="19" t="s">
         <v>59</v>
       </c>
@@ -15786,7 +15793,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="19" t="s">
         <v>275</v>
       </c>
@@ -15861,7 +15868,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="19" t="s">
         <v>277</v>
       </c>
@@ -15936,7 +15943,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="19" t="s">
         <v>279</v>
       </c>
@@ -16011,7 +16018,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="128" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
         <v>286</v>
       </c>
@@ -16088,7 +16095,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="s">
         <v>288</v>
       </c>
@@ -16166,7 +16173,7 @@
       </c>
       <c r="Z129" s="2"/>
     </row>
-    <row r="130" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
         <v>310</v>
       </c>
@@ -16244,7 +16251,7 @@
       </c>
       <c r="Z130" s="2"/>
     </row>
-    <row r="131" spans="1:26" s="38" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
         <v>66</v>
       </c>
@@ -16320,9 +16327,9 @@
       <c r="Y131" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="Z131" s="37"/>
-    </row>
-    <row r="132" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="Z131" s="31"/>
+    </row>
+    <row r="132" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="23" t="s">
         <v>336</v>
       </c>
@@ -16400,7 +16407,7 @@
       </c>
       <c r="Z132" s="2"/>
     </row>
-    <row r="133" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="23" t="s">
         <v>338</v>
       </c>
@@ -16478,7 +16485,7 @@
       </c>
       <c r="Z133" s="2"/>
     </row>
-    <row r="134" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="23" t="s">
         <v>340</v>
       </c>
@@ -16556,7 +16563,7 @@
       </c>
       <c r="Z134" s="2"/>
     </row>
-    <row r="135" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="23" t="s">
         <v>342</v>
       </c>
@@ -16634,7 +16641,7 @@
       </c>
       <c r="Z135" s="2"/>
     </row>
-    <row r="136" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="23" t="s">
         <v>344</v>
       </c>
@@ -16712,7 +16719,7 @@
       </c>
       <c r="Z136" s="2"/>
     </row>
-    <row r="137" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="23" t="s">
         <v>346</v>
       </c>
@@ -16790,7 +16797,7 @@
       </c>
       <c r="Z137" s="2"/>
     </row>
-    <row r="138" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="23" t="s">
         <v>290</v>
       </c>
@@ -16868,7 +16875,7 @@
       </c>
       <c r="Z138" s="2"/>
     </row>
-    <row r="139" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="23" t="s">
         <v>292</v>
       </c>
@@ -16946,7 +16953,7 @@
       </c>
       <c r="Z139" s="2"/>
     </row>
-    <row r="140" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="23" t="s">
         <v>294</v>
       </c>
@@ -17024,7 +17031,7 @@
       </c>
       <c r="Z140" s="2"/>
     </row>
-    <row r="141" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="23" t="s">
         <v>296</v>
       </c>
@@ -17102,7 +17109,7 @@
       </c>
       <c r="Z141" s="2"/>
     </row>
-    <row r="142" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="23" t="s">
         <v>298</v>
       </c>
@@ -17180,7 +17187,7 @@
       </c>
       <c r="Z142" s="2"/>
     </row>
-    <row r="143" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="23" t="s">
         <v>300</v>
       </c>
@@ -17258,7 +17265,7 @@
       </c>
       <c r="Z143" s="2"/>
     </row>
-    <row r="144" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="23" t="s">
         <v>302</v>
       </c>
@@ -17336,7 +17343,7 @@
       </c>
       <c r="Z144" s="2"/>
     </row>
-    <row r="145" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="23" t="s">
         <v>304</v>
       </c>
@@ -17414,7 +17421,7 @@
       </c>
       <c r="Z145" s="2"/>
     </row>
-    <row r="146" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="s">
         <v>306</v>
       </c>
@@ -17492,7 +17499,7 @@
       </c>
       <c r="Z146" s="2"/>
     </row>
-    <row r="147" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="s">
         <v>308</v>
       </c>
@@ -17570,7 +17577,7 @@
       </c>
       <c r="Z147" s="2"/>
     </row>
-    <row r="148" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="23" t="s">
         <v>312</v>
       </c>
@@ -17648,7 +17655,7 @@
       </c>
       <c r="Z148" s="2"/>
     </row>
-    <row r="149" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="23" t="s">
         <v>314</v>
       </c>
@@ -17726,7 +17733,7 @@
       </c>
       <c r="Z149" s="2"/>
     </row>
-    <row r="150" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="23" t="s">
         <v>316</v>
       </c>
@@ -17804,7 +17811,7 @@
       </c>
       <c r="Z150" s="2"/>
     </row>
-    <row r="151" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="23" t="s">
         <v>318</v>
       </c>
@@ -17882,7 +17889,7 @@
       </c>
       <c r="Z151" s="2"/>
     </row>
-    <row r="152" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="23" t="s">
         <v>320</v>
       </c>
@@ -17958,7 +17965,7 @@
       </c>
       <c r="Z152" s="2"/>
     </row>
-    <row r="153" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
         <v>322</v>
       </c>
@@ -18036,7 +18043,7 @@
       </c>
       <c r="Z153" s="2"/>
     </row>
-    <row r="154" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
         <v>324</v>
       </c>
@@ -18114,7 +18121,7 @@
       </c>
       <c r="Z154" s="2"/>
     </row>
-    <row r="155" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="23" t="s">
         <v>326</v>
       </c>
@@ -18189,7 +18196,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="156" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="23" t="s">
         <v>73</v>
       </c>
@@ -18264,7 +18271,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="157" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
         <v>329</v>
       </c>
@@ -18341,7 +18348,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="158" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
         <v>332</v>
       </c>
@@ -18418,7 +18425,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="159" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
         <v>334</v>
       </c>
@@ -18495,7 +18502,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="160" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="23" t="s">
         <v>347</v>
       </c>
@@ -18570,7 +18577,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="161" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
         <v>348</v>
       </c>
@@ -18645,7 +18652,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="162" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
         <v>349</v>
       </c>
@@ -18720,7 +18727,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
         <v>351</v>
       </c>
@@ -18795,7 +18802,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="164" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
         <v>353</v>
       </c>
@@ -18870,7 +18877,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="165" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
         <v>355</v>
       </c>
@@ -18945,7 +18952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
         <v>357</v>
       </c>
@@ -19020,7 +19027,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="167" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>359</v>
       </c>
@@ -19095,7 +19102,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="168" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
         <v>361</v>
       </c>
@@ -19170,7 +19177,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="169" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
         <v>363</v>
       </c>
@@ -19245,7 +19252,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="170" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
         <v>365</v>
       </c>
@@ -19320,7 +19327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="171" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
         <v>367</v>
       </c>
@@ -19395,7 +19402,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="172" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
         <v>369</v>
       </c>
@@ -19470,7 +19477,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="173" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
         <v>370</v>
       </c>
@@ -19545,7 +19552,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="174" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
         <v>372</v>
       </c>
@@ -19620,7 +19627,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="175" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
         <v>374</v>
       </c>
@@ -19695,7 +19702,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="176" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
         <v>376</v>
       </c>
@@ -19770,7 +19777,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
         <v>264</v>
       </c>
@@ -19845,7 +19852,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="178" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
         <v>134</v>
       </c>
@@ -19920,7 +19927,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="179" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
         <v>377</v>
       </c>
@@ -19995,7 +20002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="180" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
         <v>378</v>
       </c>
@@ -20070,7 +20077,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="181" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
         <v>379</v>
       </c>
@@ -20145,7 +20152,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="182" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="19" t="s">
         <v>381</v>
       </c>
@@ -20220,7 +20227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="183" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="19" t="s">
         <v>383</v>
       </c>
@@ -20295,7 +20302,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="184" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="19" t="s">
         <v>385</v>
       </c>
@@ -20370,7 +20377,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="185" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="19" t="s">
         <v>387</v>
       </c>
@@ -20445,7 +20452,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="186" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="19" t="s">
         <v>389</v>
       </c>
@@ -20520,7 +20527,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="187" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
         <v>390</v>
       </c>
@@ -20595,7 +20602,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="188" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
         <v>391</v>
       </c>
@@ -20670,7 +20677,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="189" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
         <v>392</v>
       </c>
@@ -20745,7 +20752,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="190" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
         <v>393</v>
       </c>
@@ -20820,7 +20827,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="191" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
         <v>395</v>
       </c>
@@ -20897,7 +20904,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="192" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
         <v>397</v>
       </c>
@@ -20972,7 +20979,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="193" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
         <v>399</v>
       </c>
@@ -21051,6 +21058,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:Y193" xr:uid="{E9FC8F81-7F97-4E33-8AE4-FE56471D62CF}"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="A1:Y193">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Reserved">
       <formula>NOT(ISERROR(SEARCH("Reserved",A1)))</formula>
@@ -21068,9 +21076,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>400</v>
       </c>
@@ -21093,7 +21101,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>407</v>
       </c>
@@ -21132,7 +21140,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21152,6 +21160,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed1bc3df-35b6-4046-a92f-d0f102935d5b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095AC27E69C8BDF408C662988E5DEDD09" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d967c290cd26da344506a5481f315d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed1bc3df-35b6-4046-a92f-d0f102935d5b" xmlns:ns3="c4672b8b-43e2-4139-8cd1-27ad03f081e7" xmlns:ns4="6dd24d01-1828-4579-8bd7-ef8e5a7c81f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e12b773f8ef9a33d5e99b91e8900b87" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="ed1bc3df-35b6-4046-a92f-d0f102935d5b"/>
@@ -21385,17 +21404,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed1bc3df-35b6-4046-a92f-d0f102935d5b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5075A188-DA7E-4928-8AD4-DB194C82EA94}">
   <ds:schemaRefs>
@@ -21405,6 +21413,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9DF1D96-BD46-446A-AC2E-6C075F1608B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="ed1bc3df-35b6-4046-a92f-d0f102935d5b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6dd24d01-1828-4579-8bd7-ef8e5a7c81f8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1795044-A6F2-4994-9DCD-76F1D2FF53CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21422,22 +21448,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9DF1D96-BD46-446A-AC2E-6C075F1608B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ed1bc3df-35b6-4046-a92f-d0f102935d5b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6dd24d01-1828-4579-8bd7-ef8e5a7c81f8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>